<commit_message>
feat(clean): docentes y estudiantes
</commit_message>
<xml_diff>
--- a/Segregaciones/Docentes_solo_desconocidos.xlsx
+++ b/Segregaciones/Docentes_solo_desconocidos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1057,6 +1057,622 @@
         <v>80</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1010751</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>DGES</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>7</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>3er. CICLO EBI</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>desconocido</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Docente</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>TALLER ARTE - ED.MUSICAL</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>41</v>
+      </c>
+      <c r="J15" t="n">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1010774</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>DGES</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>9</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>3er. CICLO EBI</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>desconocido</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Docente</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>CS.COMPUTACIONALES (Program.)</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>49</v>
+      </c>
+      <c r="J16" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1011136</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>DGES</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>8</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>3er. CICLO EBI</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>desconocido</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Docente</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>HISTORIA</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>37</v>
+      </c>
+      <c r="J17" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1011146</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>DGES</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>9</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>3er. CICLO EBI</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>desconocido</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Docente</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>TALLER PARTICIPACION JUVENIL</t>
+        </is>
+      </c>
+      <c r="I18" t="n">
+        <v>20</v>
+      </c>
+      <c r="J18" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1011147</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>DGES</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>9</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>3er. CICLO EBI</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>desconocido</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Docente</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>TALLER PARTICIPACION JUVENIL</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>41</v>
+      </c>
+      <c r="J19" t="n">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1011183</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>DGES</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>9</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>3er. CICLO EBI</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>desconocido</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Docente</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>TALLER EXPRESION ARTISTICA</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>33</v>
+      </c>
+      <c r="J20" t="n">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1011190</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>DGES</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>8</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>3er. CICLO EBI</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>desconocido</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Docente</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>ARTE - EDUCACION MUSICAL</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>27</v>
+      </c>
+      <c r="J21" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>1011196</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>DGES</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>8</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>3er. CICLO EBI</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>desconocido</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Docente</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>CS. FISICO-QUIMICA</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
+        <v>61</v>
+      </c>
+      <c r="J22" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>1011198</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>DGES</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>9</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>3er. CICLO EBI</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>desconocido</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Docente</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>INGLES</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>63</v>
+      </c>
+      <c r="J23" t="n">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>1011204</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>DGES</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>8</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>3er. CICLO EBI</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>desconocido</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Docente</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>ARTE - EDUCACION MUSICAL</t>
+        </is>
+      </c>
+      <c r="I24" t="n">
+        <v>55</v>
+      </c>
+      <c r="J24" t="n">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>1011642</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>DGES</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>8</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>3er. CICLO EBI</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>desconocido</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Docente</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>CS.COMPUTACIONALES (Tecnolog.)</t>
+        </is>
+      </c>
+      <c r="I25" t="n">
+        <v>50</v>
+      </c>
+      <c r="J25" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>1011644</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>DGES</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>9</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>3er. CICLO EBI</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>desconocido</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Docente</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>CS.COMPUTACIONALES (Program.)</t>
+        </is>
+      </c>
+      <c r="I26" t="n">
+        <v>42</v>
+      </c>
+      <c r="J26" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>1011648</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>DGES</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>8</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>3er. CICLO EBI</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>desconocido</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Docente</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>HISTORIA</t>
+        </is>
+      </c>
+      <c r="I27" t="n">
+        <v>47</v>
+      </c>
+      <c r="J27" t="n">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>1011717</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>DGES</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>7</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>3er. CICLO EBI</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>desconocido</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Docente</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>LENGUA ESPAÑOLA</t>
+        </is>
+      </c>
+      <c r="I28" t="n">
+        <v>54</v>
+      </c>
+      <c r="J28" t="n">
+        <v>152</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
arreglo pregunta 2 que no corria
</commit_message>
<xml_diff>
--- a/Segregaciones/Docentes_solo_desconocidos.xlsx
+++ b/Segregaciones/Docentes_solo_desconocidos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,15 +471,10 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>materia</t>
+          <t>edad</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>edad</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>id_centro</t>
         </is>
@@ -517,15 +512,10 @@
           <t>Docente</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>LENGUA ESPAÑOLA</t>
-        </is>
+      <c r="H2" t="n">
+        <v>35</v>
       </c>
       <c r="I2" t="n">
-        <v>35</v>
-      </c>
-      <c r="J2" t="n">
         <v>25</v>
       </c>
     </row>
@@ -561,15 +551,10 @@
           <t>Docente</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>COMUNICACION Y SOCIEDAD</t>
-        </is>
+      <c r="H3" t="n">
+        <v>35</v>
       </c>
       <c r="I3" t="n">
-        <v>35</v>
-      </c>
-      <c r="J3" t="n">
         <v>25</v>
       </c>
     </row>
@@ -605,15 +590,10 @@
           <t>Docente</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>LENGUA ESPAÑOLA</t>
-        </is>
+      <c r="H4" t="n">
+        <v>35</v>
       </c>
       <c r="I4" t="n">
-        <v>35</v>
-      </c>
-      <c r="J4" t="n">
         <v>219</v>
       </c>
     </row>
@@ -649,15 +629,10 @@
           <t>Docente</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>GEOGRAFIA</t>
-        </is>
+      <c r="H5" t="n">
+        <v>42</v>
       </c>
       <c r="I5" t="n">
-        <v>42</v>
-      </c>
-      <c r="J5" t="n">
         <v>49</v>
       </c>
     </row>
@@ -693,15 +668,10 @@
           <t>Docente</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>EDUCACION FISICA Y RECREACION</t>
-        </is>
+      <c r="H6" t="n">
+        <v>59</v>
       </c>
       <c r="I6" t="n">
-        <v>59</v>
-      </c>
-      <c r="J6" t="n">
         <v>64</v>
       </c>
     </row>
@@ -737,15 +707,10 @@
           <t>Docente</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>EDUCACION FISICA Y RECREACION</t>
-        </is>
+      <c r="H7" t="n">
+        <v>59</v>
       </c>
       <c r="I7" t="n">
-        <v>59</v>
-      </c>
-      <c r="J7" t="n">
         <v>64</v>
       </c>
     </row>
@@ -781,15 +746,10 @@
           <t>Docente</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>COMUNICACION Y SOCIEDAD</t>
-        </is>
+      <c r="H8" t="n">
+        <v>41</v>
       </c>
       <c r="I8" t="n">
-        <v>41</v>
-      </c>
-      <c r="J8" t="n">
         <v>146</v>
       </c>
     </row>
@@ -825,15 +785,10 @@
           <t>Docente</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>COMUNICACION Y SOCIEDAD</t>
-        </is>
+      <c r="H9" t="n">
+        <v>41</v>
       </c>
       <c r="I9" t="n">
-        <v>41</v>
-      </c>
-      <c r="J9" t="n">
         <v>146</v>
       </c>
     </row>
@@ -869,15 +824,10 @@
           <t>Docente</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>LITERATURA</t>
-        </is>
+      <c r="H10" t="n">
+        <v>41</v>
       </c>
       <c r="I10" t="n">
-        <v>41</v>
-      </c>
-      <c r="J10" t="n">
         <v>146</v>
       </c>
     </row>
@@ -913,15 +863,10 @@
           <t>Docente</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>ARTE - EDUCACION MUSICAL</t>
-        </is>
+      <c r="H11" t="n">
+        <v>40</v>
       </c>
       <c r="I11" t="n">
-        <v>40</v>
-      </c>
-      <c r="J11" t="n">
         <v>212</v>
       </c>
     </row>
@@ -957,15 +902,10 @@
           <t>Docente</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>TALLER ARTE - ED.MUSICAL</t>
-        </is>
+      <c r="H12" t="n">
+        <v>40</v>
       </c>
       <c r="I12" t="n">
-        <v>40</v>
-      </c>
-      <c r="J12" t="n">
         <v>212</v>
       </c>
     </row>
@@ -1001,15 +941,10 @@
           <t>Docente</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>ARTE - EDUCACION MUSICAL</t>
-        </is>
+      <c r="H13" t="n">
+        <v>40</v>
       </c>
       <c r="I13" t="n">
-        <v>40</v>
-      </c>
-      <c r="J13" t="n">
         <v>212</v>
       </c>
     </row>
@@ -1045,15 +980,10 @@
           <t>Docente</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>CS. DEL AMBIENTE - GEOGRAFIA</t>
-        </is>
+      <c r="H14" t="n">
+        <v>42</v>
       </c>
       <c r="I14" t="n">
-        <v>42</v>
-      </c>
-      <c r="J14" t="n">
         <v>80</v>
       </c>
     </row>
@@ -1089,15 +1019,10 @@
           <t>Docente</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>TALLER ARTE - ED.MUSICAL</t>
-        </is>
+      <c r="H15" t="n">
+        <v>41</v>
       </c>
       <c r="I15" t="n">
-        <v>41</v>
-      </c>
-      <c r="J15" t="n">
         <v>136</v>
       </c>
     </row>
@@ -1133,15 +1058,10 @@
           <t>Docente</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>CS.COMPUTACIONALES (Program.)</t>
-        </is>
+      <c r="H16" t="n">
+        <v>49</v>
       </c>
       <c r="I16" t="n">
-        <v>49</v>
-      </c>
-      <c r="J16" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1177,15 +1097,10 @@
           <t>Docente</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>HISTORIA</t>
-        </is>
+      <c r="H17" t="n">
+        <v>37</v>
       </c>
       <c r="I17" t="n">
-        <v>37</v>
-      </c>
-      <c r="J17" t="n">
         <v>97</v>
       </c>
     </row>
@@ -1221,15 +1136,10 @@
           <t>Docente</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>TALLER PARTICIPACION JUVENIL</t>
-        </is>
+      <c r="H18" t="n">
+        <v>20</v>
       </c>
       <c r="I18" t="n">
-        <v>20</v>
-      </c>
-      <c r="J18" t="n">
         <v>59</v>
       </c>
     </row>
@@ -1265,15 +1175,10 @@
           <t>Docente</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>TALLER PARTICIPACION JUVENIL</t>
-        </is>
+      <c r="H19" t="n">
+        <v>41</v>
       </c>
       <c r="I19" t="n">
-        <v>41</v>
-      </c>
-      <c r="J19" t="n">
         <v>206</v>
       </c>
     </row>
@@ -1309,15 +1214,10 @@
           <t>Docente</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>TALLER EXPRESION ARTISTICA</t>
-        </is>
+      <c r="H20" t="n">
+        <v>33</v>
       </c>
       <c r="I20" t="n">
-        <v>33</v>
-      </c>
-      <c r="J20" t="n">
         <v>144</v>
       </c>
     </row>
@@ -1353,15 +1253,10 @@
           <t>Docente</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>ARTE - EDUCACION MUSICAL</t>
-        </is>
+      <c r="H21" t="n">
+        <v>27</v>
       </c>
       <c r="I21" t="n">
-        <v>27</v>
-      </c>
-      <c r="J21" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1397,15 +1292,10 @@
           <t>Docente</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>CS. FISICO-QUIMICA</t>
-        </is>
+      <c r="H22" t="n">
+        <v>61</v>
       </c>
       <c r="I22" t="n">
-        <v>61</v>
-      </c>
-      <c r="J22" t="n">
         <v>75</v>
       </c>
     </row>
@@ -1441,15 +1331,10 @@
           <t>Docente</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>INGLES</t>
-        </is>
+      <c r="H23" t="n">
+        <v>63</v>
       </c>
       <c r="I23" t="n">
-        <v>63</v>
-      </c>
-      <c r="J23" t="n">
         <v>102</v>
       </c>
     </row>
@@ -1485,15 +1370,10 @@
           <t>Docente</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>ARTE - EDUCACION MUSICAL</t>
-        </is>
+      <c r="H24" t="n">
+        <v>55</v>
       </c>
       <c r="I24" t="n">
-        <v>55</v>
-      </c>
-      <c r="J24" t="n">
         <v>207</v>
       </c>
     </row>
@@ -1529,15 +1409,10 @@
           <t>Docente</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>CS.COMPUTACIONALES (Tecnolog.)</t>
-        </is>
+      <c r="H25" t="n">
+        <v>50</v>
       </c>
       <c r="I25" t="n">
-        <v>50</v>
-      </c>
-      <c r="J25" t="n">
         <v>61</v>
       </c>
     </row>
@@ -1573,15 +1448,10 @@
           <t>Docente</t>
         </is>
       </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>CS.COMPUTACIONALES (Program.)</t>
-        </is>
+      <c r="H26" t="n">
+        <v>42</v>
       </c>
       <c r="I26" t="n">
-        <v>42</v>
-      </c>
-      <c r="J26" t="n">
         <v>56</v>
       </c>
     </row>
@@ -1617,15 +1487,10 @@
           <t>Docente</t>
         </is>
       </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>HISTORIA</t>
-        </is>
+      <c r="H27" t="n">
+        <v>47</v>
       </c>
       <c r="I27" t="n">
-        <v>47</v>
-      </c>
-      <c r="J27" t="n">
         <v>145</v>
       </c>
     </row>
@@ -1661,15 +1526,10 @@
           <t>Docente</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>LENGUA ESPAÑOLA</t>
-        </is>
+      <c r="H28" t="n">
+        <v>54</v>
       </c>
       <c r="I28" t="n">
-        <v>54</v>
-      </c>
-      <c r="J28" t="n">
         <v>152</v>
       </c>
     </row>

</xml_diff>